<commit_message>
refactoring summary (add unit) and handle duplicate values
</commit_message>
<xml_diff>
--- a/dataset/Material.xlsx
+++ b/dataset/Material.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/benjaminkauffmann/Desktop/Azasimul/azasimul/dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A45676C-E438-7747-89B6-736C14AC2D23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D108DA1-7582-F84F-BE03-251163F4213A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20920" yWindow="500" windowWidth="17480" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="221">
   <si>
     <t>Portal</t>
   </si>
@@ -732,6 +732,9 @@
   </si>
   <si>
     <t>End</t>
+  </si>
+  <si>
+    <t>date</t>
   </si>
 </sst>
 </file>
@@ -1933,7 +1936,7 @@
   <dimension ref="A1:F39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1978,7 +1981,9 @@
       <c r="B4" s="175">
         <v>44849</v>
       </c>
-      <c r="C4" s="97"/>
+      <c r="C4" s="97" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="5" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="163" t="s">
@@ -1987,7 +1992,9 @@
       <c r="B5" s="176">
         <v>-6.3E-2</v>
       </c>
-      <c r="C5" s="97"/>
+      <c r="C5" s="97" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="6" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="97" t="s">
@@ -2023,7 +2030,9 @@
       <c r="B9" s="175">
         <v>44849</v>
       </c>
-      <c r="C9" s="97"/>
+      <c r="C9" s="97" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="10" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="97" t="s">
@@ -2032,7 +2041,9 @@
       <c r="B10" s="175">
         <v>48502</v>
       </c>
-      <c r="C10" s="97"/>
+      <c r="C10" s="97" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="11" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="97"/>

</xml_diff>

<commit_message>
add FOR directive to output
</commit_message>
<xml_diff>
--- a/dataset/Material.xlsx
+++ b/dataset/Material.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/benjaminkauffmann/Desktop/Azasimul/azasimul/dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D108DA1-7582-F84F-BE03-251163F4213A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{438C1E45-81E7-1243-9430-98708589CB74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20920" yWindow="500" windowWidth="17480" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20920" yWindow="500" windowWidth="17480" windowHeight="15540" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -692,9 +692,6 @@
     <t>Manufacturing</t>
   </si>
   <si>
-    <t>cost</t>
-  </si>
-  <si>
     <t>Project Type</t>
   </si>
   <si>
@@ -735,6 +732,9 @@
   </si>
   <si>
     <t>date</t>
+  </si>
+  <si>
+    <t>$</t>
   </si>
 </sst>
 </file>
@@ -1935,8 +1935,8 @@
   </sheetPr>
   <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1949,45 +1949,45 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="97" t="s">
+        <v>206</v>
+      </c>
+      <c r="B1" s="97" t="s">
         <v>207</v>
-      </c>
-      <c r="B1" s="97" t="s">
-        <v>208</v>
       </c>
       <c r="C1" s="97"/>
     </row>
     <row r="2" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="97" t="s">
+        <v>208</v>
+      </c>
+      <c r="B2" s="97" t="s">
         <v>209</v>
-      </c>
-      <c r="B2" s="97" t="s">
-        <v>210</v>
       </c>
       <c r="C2" s="97"/>
     </row>
     <row r="3" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="97" t="s">
+        <v>210</v>
+      </c>
+      <c r="B3" s="97" t="s">
         <v>211</v>
-      </c>
-      <c r="B3" s="97" t="s">
-        <v>212</v>
       </c>
       <c r="C3" s="97"/>
     </row>
     <row r="4" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="97" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B4" s="175">
         <v>44849</v>
       </c>
       <c r="C4" s="97" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="163" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B5" s="176">
         <v>-6.3E-2</v>
@@ -1998,7 +1998,7 @@
     </row>
     <row r="6" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="97" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B6" s="162">
         <v>5</v>
@@ -2007,7 +2007,7 @@
     </row>
     <row r="7" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="97" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B7" s="162">
         <v>150</v>
@@ -2016,7 +2016,7 @@
     </row>
     <row r="8" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="97" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B8" s="162">
         <v>24</v>
@@ -2025,24 +2025,24 @@
     </row>
     <row r="9" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="97" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B9" s="175">
         <v>44849</v>
       </c>
       <c r="C9" s="97" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="97" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B10" s="175">
         <v>48502</v>
       </c>
       <c r="C10" s="97" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4105,7 +4105,9 @@
   </sheetPr>
   <dimension ref="A1:M41"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4425,10 +4427,10 @@
         <v>178</v>
       </c>
       <c r="I18" s="139" t="s">
-        <v>206</v>
+        <v>220</v>
       </c>
       <c r="J18" s="139" t="s">
-        <v>206</v>
+        <v>220</v>
       </c>
       <c r="K18" s="140"/>
       <c r="L18" s="140"/>
@@ -5626,7 +5628,7 @@
   </sheetPr>
   <dimension ref="A1:P41"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>